<commit_message>
works with 95% correctness
</commit_message>
<xml_diff>
--- a/bbtnbc2.xlsx
+++ b/bbtnbc2.xlsx
@@ -112,11 +112,11 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="16"/>
+      <color indexed="17"/>
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,8 +159,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -280,99 +286,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -406,10 +326,10 @@
     <xf numFmtId="49" fontId="4" fillId="7" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -430,100 +350,40 @@
     <xf numFmtId="49" fontId="3" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -550,6 +410,7 @@
       <rgbColor rgb="ffe97132"/>
       <rgbColor rgb="ffa02b93"/>
       <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaeaeae"/>
     </indexedColors>
   </colors>
@@ -749,17 +610,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="19050" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -786,10 +647,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Aptos Narrow"/>
-            <a:ea typeface="Aptos Narrow"/>
-            <a:cs typeface="Aptos Narrow"/>
-            <a:sym typeface="Aptos Narrow"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1028,12 +889,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="19050" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1310,7 +1171,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1337,10 +1198,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Aptos Narrow"/>
-            <a:ea typeface="Aptos Narrow"/>
-            <a:cs typeface="Aptos Narrow"/>
-            <a:sym typeface="Aptos Narrow"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1582,7 +1443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:X102"/>
+  <dimension ref="A1:X82"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -5441,526 +5302,6 @@
       <c r="W82" s="12"/>
       <c r="X82" s="12"/>
     </row>
-    <row r="83" ht="17" customHeight="1">
-      <c r="A83" s="31"/>
-      <c r="B83" s="31"/>
-      <c r="C83" s="32"/>
-      <c r="D83" s="32"/>
-      <c r="E83" s="33"/>
-      <c r="F83" s="32"/>
-      <c r="G83" s="32"/>
-      <c r="H83" s="32"/>
-      <c r="I83" s="32"/>
-      <c r="J83" s="33"/>
-      <c r="K83" s="34"/>
-      <c r="L83" s="12"/>
-      <c r="M83" s="12"/>
-      <c r="N83" s="12"/>
-      <c r="O83" s="12"/>
-      <c r="P83" s="12"/>
-      <c r="Q83" s="12"/>
-      <c r="R83" s="12"/>
-      <c r="S83" s="12"/>
-      <c r="T83" s="12"/>
-      <c r="U83" s="12"/>
-      <c r="V83" s="12"/>
-      <c r="W83" s="12"/>
-      <c r="X83" s="12"/>
-    </row>
-    <row r="84" ht="16" customHeight="1">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="12"/>
-      <c r="K84" s="12"/>
-      <c r="L84" s="12"/>
-      <c r="M84" s="12"/>
-      <c r="N84" s="12"/>
-      <c r="O84" s="12"/>
-      <c r="P84" s="12"/>
-      <c r="Q84" s="12"/>
-      <c r="R84" s="12"/>
-      <c r="S84" s="12"/>
-      <c r="T84" s="12"/>
-      <c r="U84" s="12"/>
-      <c r="V84" s="12"/>
-      <c r="W84" s="12"/>
-      <c r="X84" s="12"/>
-    </row>
-    <row r="85" ht="16" customHeight="1">
-      <c r="A85" s="12"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="12"/>
-      <c r="I85" s="12"/>
-      <c r="J85" s="12"/>
-      <c r="K85" s="12"/>
-      <c r="L85" s="12"/>
-      <c r="M85" s="12"/>
-      <c r="N85" s="12"/>
-      <c r="O85" s="12"/>
-      <c r="P85" s="12"/>
-      <c r="Q85" s="12"/>
-      <c r="R85" s="12"/>
-      <c r="S85" s="12"/>
-      <c r="T85" s="12"/>
-      <c r="U85" s="12"/>
-      <c r="V85" s="12"/>
-      <c r="W85" s="12"/>
-      <c r="X85" s="12"/>
-    </row>
-    <row r="86" ht="16" customHeight="1">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="12"/>
-      <c r="I86" s="12"/>
-      <c r="J86" s="12"/>
-      <c r="K86" s="12"/>
-      <c r="L86" s="12"/>
-      <c r="M86" s="12"/>
-      <c r="N86" s="12"/>
-      <c r="O86" s="12"/>
-      <c r="P86" s="12"/>
-      <c r="Q86" s="12"/>
-      <c r="R86" s="12"/>
-      <c r="S86" s="12"/>
-      <c r="T86" s="12"/>
-      <c r="U86" s="12"/>
-      <c r="V86" s="12"/>
-      <c r="W86" s="12"/>
-      <c r="X86" s="12"/>
-    </row>
-    <row r="87" ht="16" customHeight="1">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="12"/>
-      <c r="H87" s="12"/>
-      <c r="I87" s="12"/>
-      <c r="J87" s="12"/>
-      <c r="K87" s="12"/>
-      <c r="L87" s="12"/>
-      <c r="M87" s="12"/>
-      <c r="N87" s="12"/>
-      <c r="O87" s="12"/>
-      <c r="P87" s="12"/>
-      <c r="Q87" s="12"/>
-      <c r="R87" s="12"/>
-      <c r="S87" s="12"/>
-      <c r="T87" s="12"/>
-      <c r="U87" s="12"/>
-      <c r="V87" s="12"/>
-      <c r="W87" s="12"/>
-      <c r="X87" s="12"/>
-    </row>
-    <row r="88" ht="16" customHeight="1">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="12"/>
-      <c r="I88" s="12"/>
-      <c r="J88" s="12"/>
-      <c r="K88" s="12"/>
-      <c r="L88" s="12"/>
-      <c r="M88" s="12"/>
-      <c r="N88" s="12"/>
-      <c r="O88" s="12"/>
-      <c r="P88" s="12"/>
-      <c r="Q88" s="12"/>
-      <c r="R88" s="12"/>
-      <c r="S88" s="12"/>
-      <c r="T88" s="12"/>
-      <c r="U88" s="12"/>
-      <c r="V88" s="12"/>
-      <c r="W88" s="12"/>
-      <c r="X88" s="12"/>
-    </row>
-    <row r="89" ht="16" customHeight="1">
-      <c r="A89" s="12"/>
-      <c r="B89" s="12"/>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
-      <c r="G89" s="12"/>
-      <c r="H89" s="12"/>
-      <c r="I89" s="12"/>
-      <c r="J89" s="12"/>
-      <c r="K89" s="12"/>
-      <c r="L89" s="12"/>
-      <c r="M89" s="12"/>
-      <c r="N89" s="12"/>
-      <c r="O89" s="12"/>
-      <c r="P89" s="12"/>
-      <c r="Q89" s="12"/>
-      <c r="R89" s="12"/>
-      <c r="S89" s="12"/>
-      <c r="T89" s="12"/>
-      <c r="U89" s="12"/>
-      <c r="V89" s="12"/>
-      <c r="W89" s="12"/>
-      <c r="X89" s="12"/>
-    </row>
-    <row r="90" ht="16" customHeight="1">
-      <c r="A90" s="12"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="12"/>
-      <c r="H90" s="12"/>
-      <c r="I90" s="12"/>
-      <c r="J90" s="12"/>
-      <c r="K90" s="12"/>
-      <c r="L90" s="12"/>
-      <c r="M90" s="12"/>
-      <c r="N90" s="12"/>
-      <c r="O90" s="12"/>
-      <c r="P90" s="12"/>
-      <c r="Q90" s="12"/>
-      <c r="R90" s="12"/>
-      <c r="S90" s="12"/>
-      <c r="T90" s="12"/>
-      <c r="U90" s="12"/>
-      <c r="V90" s="12"/>
-      <c r="W90" s="12"/>
-      <c r="X90" s="12"/>
-    </row>
-    <row r="91" ht="16" customHeight="1">
-      <c r="A91" s="12"/>
-      <c r="B91" s="12"/>
-      <c r="C91" s="12"/>
-      <c r="D91" s="12"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="12"/>
-      <c r="H91" s="12"/>
-      <c r="I91" s="12"/>
-      <c r="J91" s="12"/>
-      <c r="K91" s="12"/>
-      <c r="L91" s="12"/>
-      <c r="M91" s="12"/>
-      <c r="N91" s="12"/>
-      <c r="O91" s="12"/>
-      <c r="P91" s="12"/>
-      <c r="Q91" s="12"/>
-      <c r="R91" s="12"/>
-      <c r="S91" s="12"/>
-      <c r="T91" s="12"/>
-      <c r="U91" s="12"/>
-      <c r="V91" s="12"/>
-      <c r="W91" s="12"/>
-      <c r="X91" s="12"/>
-    </row>
-    <row r="92" ht="17" customHeight="1">
-      <c r="A92" s="32"/>
-      <c r="B92" s="32"/>
-      <c r="C92" s="12"/>
-      <c r="D92" s="12"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="12"/>
-      <c r="H92" s="12"/>
-      <c r="I92" s="12"/>
-      <c r="J92" s="12"/>
-      <c r="K92" s="12"/>
-      <c r="L92" s="12"/>
-      <c r="M92" s="12"/>
-      <c r="N92" s="12"/>
-      <c r="O92" s="12"/>
-      <c r="P92" s="12"/>
-      <c r="Q92" s="34"/>
-      <c r="R92" s="12"/>
-      <c r="S92" s="12"/>
-      <c r="T92" s="12"/>
-      <c r="U92" s="12"/>
-      <c r="V92" s="12"/>
-      <c r="W92" s="12"/>
-      <c r="X92" s="12"/>
-    </row>
-    <row r="93" ht="17" customHeight="1">
-      <c r="A93" s="32"/>
-      <c r="B93" s="32"/>
-      <c r="C93" s="32"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="12"/>
-      <c r="I93" s="12"/>
-      <c r="J93" s="12"/>
-      <c r="K93" s="12"/>
-      <c r="L93" s="12"/>
-      <c r="M93" s="12"/>
-      <c r="N93" s="12"/>
-      <c r="O93" s="32"/>
-      <c r="P93" s="12"/>
-      <c r="Q93" s="34"/>
-      <c r="R93" s="12"/>
-      <c r="S93" s="12"/>
-      <c r="T93" s="12"/>
-      <c r="U93" s="12"/>
-      <c r="V93" s="12"/>
-      <c r="W93" s="12"/>
-      <c r="X93" s="12"/>
-    </row>
-    <row r="94" ht="17" customHeight="1">
-      <c r="A94" s="32"/>
-      <c r="B94" s="32"/>
-      <c r="C94" s="32"/>
-      <c r="D94" s="12"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="12"/>
-      <c r="I94" s="12"/>
-      <c r="J94" s="12"/>
-      <c r="K94" s="12"/>
-      <c r="L94" s="12"/>
-      <c r="M94" s="35"/>
-      <c r="N94" s="35"/>
-      <c r="O94" s="35"/>
-      <c r="P94" s="35"/>
-      <c r="Q94" s="36"/>
-      <c r="R94" s="37"/>
-      <c r="S94" s="37"/>
-      <c r="T94" s="37"/>
-      <c r="U94" s="37"/>
-      <c r="V94" s="37"/>
-      <c r="W94" s="12"/>
-      <c r="X94" s="12"/>
-    </row>
-    <row r="95" ht="16" customHeight="1">
-      <c r="A95" s="34"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="34"/>
-      <c r="D95" s="34"/>
-      <c r="E95" s="34"/>
-      <c r="F95" s="34"/>
-      <c r="G95" s="34"/>
-      <c r="H95" s="34"/>
-      <c r="I95" s="34"/>
-      <c r="J95" s="34"/>
-      <c r="K95" s="34"/>
-      <c r="L95" s="38"/>
-      <c r="M95" s="39"/>
-      <c r="N95" s="39"/>
-      <c r="O95" s="39"/>
-      <c r="P95" s="40"/>
-      <c r="Q95" s="41"/>
-      <c r="R95" s="42"/>
-      <c r="S95" s="43"/>
-      <c r="T95" s="43"/>
-      <c r="U95" s="44"/>
-      <c r="V95" s="45"/>
-      <c r="W95" s="19"/>
-      <c r="X95" s="12"/>
-    </row>
-    <row r="96" ht="17" customHeight="1">
-      <c r="A96" s="32"/>
-      <c r="B96" s="32"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="32"/>
-      <c r="E96" s="32"/>
-      <c r="F96" s="46"/>
-      <c r="G96" s="47"/>
-      <c r="H96" s="47"/>
-      <c r="I96" s="47"/>
-      <c r="J96" s="47"/>
-      <c r="K96" s="47"/>
-      <c r="L96" s="48"/>
-      <c r="M96" s="26"/>
-      <c r="N96" s="26"/>
-      <c r="O96" s="26"/>
-      <c r="P96" s="26"/>
-      <c r="Q96" s="26"/>
-      <c r="R96" s="26"/>
-      <c r="S96" s="26"/>
-      <c r="T96" s="26"/>
-      <c r="U96" s="26"/>
-      <c r="V96" s="26"/>
-      <c r="W96" s="49"/>
-      <c r="X96" s="12"/>
-    </row>
-    <row r="97" ht="17" customHeight="1">
-      <c r="A97" s="32"/>
-      <c r="B97" s="32"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="32"/>
-      <c r="F97" s="32"/>
-      <c r="G97" s="32"/>
-      <c r="H97" s="32"/>
-      <c r="I97" s="32"/>
-      <c r="J97" s="32"/>
-      <c r="K97" s="32"/>
-      <c r="L97" s="38"/>
-      <c r="M97" s="26"/>
-      <c r="N97" s="26"/>
-      <c r="O97" s="26"/>
-      <c r="P97" s="26"/>
-      <c r="Q97" s="26"/>
-      <c r="R97" s="26"/>
-      <c r="S97" s="26"/>
-      <c r="T97" s="26"/>
-      <c r="U97" s="26"/>
-      <c r="V97" s="26"/>
-      <c r="W97" s="49"/>
-      <c r="X97" s="12"/>
-    </row>
-    <row r="98" ht="17" customHeight="1">
-      <c r="A98" s="32"/>
-      <c r="B98" s="32"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="32"/>
-      <c r="E98" s="32"/>
-      <c r="F98" s="32"/>
-      <c r="G98" s="32"/>
-      <c r="H98" s="32"/>
-      <c r="I98" s="32"/>
-      <c r="J98" s="32"/>
-      <c r="K98" s="32"/>
-      <c r="L98" s="38"/>
-      <c r="M98" s="26"/>
-      <c r="N98" s="26"/>
-      <c r="O98" s="26"/>
-      <c r="P98" s="26"/>
-      <c r="Q98" s="26"/>
-      <c r="R98" s="26"/>
-      <c r="S98" s="26"/>
-      <c r="T98" s="26"/>
-      <c r="U98" s="26"/>
-      <c r="V98" s="26"/>
-      <c r="W98" s="49"/>
-      <c r="X98" s="12"/>
-    </row>
-    <row r="99" ht="17" customHeight="1">
-      <c r="A99" s="32"/>
-      <c r="B99" s="32"/>
-      <c r="C99" s="12"/>
-      <c r="D99" s="32"/>
-      <c r="E99" s="32"/>
-      <c r="F99" s="32"/>
-      <c r="G99" s="32"/>
-      <c r="H99" s="32"/>
-      <c r="I99" s="32"/>
-      <c r="J99" s="32"/>
-      <c r="K99" s="32"/>
-      <c r="L99" s="38"/>
-      <c r="M99" s="26"/>
-      <c r="N99" s="26"/>
-      <c r="O99" s="26"/>
-      <c r="P99" s="26"/>
-      <c r="Q99" s="26"/>
-      <c r="R99" s="26"/>
-      <c r="S99" s="26"/>
-      <c r="T99" s="26"/>
-      <c r="U99" s="26"/>
-      <c r="V99" s="26"/>
-      <c r="W99" s="49"/>
-      <c r="X99" s="12"/>
-    </row>
-    <row r="100" ht="17" customHeight="1">
-      <c r="A100" s="32"/>
-      <c r="B100" s="32"/>
-      <c r="C100" s="12"/>
-      <c r="D100" s="32"/>
-      <c r="E100" s="32"/>
-      <c r="F100" s="32"/>
-      <c r="G100" s="32"/>
-      <c r="H100" s="32"/>
-      <c r="I100" s="32"/>
-      <c r="J100" s="32"/>
-      <c r="K100" s="32"/>
-      <c r="L100" s="38"/>
-      <c r="M100" s="26"/>
-      <c r="N100" s="26"/>
-      <c r="O100" s="26"/>
-      <c r="P100" s="26"/>
-      <c r="Q100" s="26"/>
-      <c r="R100" s="26"/>
-      <c r="S100" s="26"/>
-      <c r="T100" s="26"/>
-      <c r="U100" s="26"/>
-      <c r="V100" s="26"/>
-      <c r="W100" s="49"/>
-      <c r="X100" s="12"/>
-    </row>
-    <row r="101" ht="17" customHeight="1">
-      <c r="A101" s="32"/>
-      <c r="B101" s="32"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="32"/>
-      <c r="E101" s="32"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="32"/>
-      <c r="H101" s="32"/>
-      <c r="I101" s="32"/>
-      <c r="J101" s="12"/>
-      <c r="K101" s="12"/>
-      <c r="L101" s="38"/>
-      <c r="M101" s="50"/>
-      <c r="N101" s="50"/>
-      <c r="O101" s="50"/>
-      <c r="P101" s="50"/>
-      <c r="Q101" s="50"/>
-      <c r="R101" s="50"/>
-      <c r="S101" s="50"/>
-      <c r="T101" s="50"/>
-      <c r="U101" s="50"/>
-      <c r="V101" s="50"/>
-      <c r="W101" s="49"/>
-      <c r="X101" s="12"/>
-    </row>
-    <row r="102" ht="17" customHeight="1">
-      <c r="A102" s="32"/>
-      <c r="B102" s="32"/>
-      <c r="C102" s="12"/>
-      <c r="D102" s="32"/>
-      <c r="E102" s="32"/>
-      <c r="F102" s="32"/>
-      <c r="G102" s="32"/>
-      <c r="H102" s="32"/>
-      <c r="I102" s="32"/>
-      <c r="J102" s="12"/>
-      <c r="K102" s="12"/>
-      <c r="L102" s="38"/>
-      <c r="M102" s="47"/>
-      <c r="N102" s="47"/>
-      <c r="O102" s="47"/>
-      <c r="P102" s="47"/>
-      <c r="Q102" s="47"/>
-      <c r="R102" s="47"/>
-      <c r="S102" s="47"/>
-      <c r="T102" s="47"/>
-      <c r="U102" s="47"/>
-      <c r="V102" s="47"/>
-      <c r="W102" s="49"/>
-      <c r="X102" s="12"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>

</xml_diff>